<commit_message>
Adding the newly generated images in 9th folder
</commit_message>
<xml_diff>
--- a/9_article1_FigsTables/Tables_data/Cases_par_data_all_ex.xlsx
+++ b/9_article1_FigsTables/Tables_data/Cases_par_data_all_ex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\datamshapratirupa\9_article1_FigsTables\Tables_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B262CD7A-B399-4539-93BA-270B6339397B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C71B1F7-ED53-48C6-B3D0-40B46A932B53}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9030" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,11 +17,12 @@
     <sheet name="data_tab" sheetId="4" r:id="rId2"/>
     <sheet name="prev_sim_params" sheetId="6" r:id="rId3"/>
     <sheet name="data_lit" sheetId="5" r:id="rId4"/>
+    <sheet name="data_final" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">Raw_data!$A$1:$M$26</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -32,6 +33,64 @@
   </authors>
   <commentList>
     <comment ref="G3" authorId="0" shapeId="0" xr:uid="{706D27D8-4914-409A-BBB8-621E014BAA8B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Radhakrishna Bangalore Lakshmiprasad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Check values once more! - Refer to the table used</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Radhakrishna Bangalore Lakshmiprasad</author>
+  </authors>
+  <commentList>
+    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{421F3332-C293-4514-8427-633309BC6AC6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Radhakrishna Bangalore Lakshmiprasad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Check values once more! - Refer to the table used</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{BD8532B6-4044-4885-A619-66490AB1F09E}">
       <text>
         <r>
           <rPr>
@@ -71,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="376">
   <si>
     <t>Column1</t>
   </si>
@@ -1214,6 +1273,24 @@
   </si>
   <si>
     <t xml:space="preserve">0.005 </t>
+  </si>
+  <si>
+    <t>0.1 - 0.2</t>
+  </si>
+  <si>
+    <t>0.3 - 0.8</t>
+  </si>
+  <si>
+    <t>0.03 - 0.12</t>
+  </si>
+  <si>
+    <t>Within range</t>
+  </si>
+  <si>
+    <t>Higher</t>
+  </si>
+  <si>
+    <t>Lower than expected</t>
   </si>
 </sst>
 </file>
@@ -1445,7 +1522,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1637,8 +1714,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="38">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -2139,6 +2252,119 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2184,7 +2410,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2222,45 +2448,6 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2329,6 +2516,123 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="34" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="34" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4923,7 +5227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" activeCellId="1" sqref="B4:B31 J4:L31"/>
     </sheetView>
   </sheetViews>
@@ -4943,22 +5247,22 @@
       <c r="B4" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="39" t="s">
         <v>200</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="20" t="s">
+      <c r="D4" s="40"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="39" t="s">
         <v>201</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="20" t="s">
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="39" t="s">
         <v>202</v>
       </c>
-      <c r="K4" s="21"/>
-      <c r="L4" s="22"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="41"/>
     </row>
     <row r="5" spans="2:12" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6"/>
@@ -5024,7 +5328,7 @@
       <c r="K6" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="L6" s="42" t="s">
         <v>219</v>
       </c>
     </row>
@@ -5059,7 +5363,7 @@
       <c r="K7" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="L7" s="15"/>
+      <c r="L7" s="43"/>
     </row>
     <row r="8" spans="2:12" ht="143.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
@@ -5092,7 +5396,7 @@
       <c r="K8" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="L8" s="16" t="s">
+      <c r="L8" s="44" t="s">
         <v>225</v>
       </c>
     </row>
@@ -5127,7 +5431,7 @@
       <c r="K9" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="L9" s="17"/>
+      <c r="L9" s="45"/>
     </row>
     <row r="10" spans="2:12" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
@@ -5160,7 +5464,7 @@
       <c r="K10" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="L10" s="18" t="s">
+      <c r="L10" s="37" t="s">
         <v>234</v>
       </c>
     </row>
@@ -5195,7 +5499,7 @@
       <c r="K11" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="L11" s="19"/>
+      <c r="L11" s="38"/>
     </row>
     <row r="12" spans="2:12" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
@@ -5228,7 +5532,7 @@
       <c r="K12" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="L12" s="16" t="s">
+      <c r="L12" s="44" t="s">
         <v>249</v>
       </c>
     </row>
@@ -5263,7 +5567,7 @@
       <c r="K13" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="L13" s="17"/>
+      <c r="L13" s="45"/>
     </row>
     <row r="14" spans="2:12" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
@@ -5296,7 +5600,7 @@
       <c r="K14" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="L14" s="18" t="s">
+      <c r="L14" s="37" t="s">
         <v>261</v>
       </c>
     </row>
@@ -5331,7 +5635,7 @@
       <c r="K15" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="L15" s="19"/>
+      <c r="L15" s="38"/>
     </row>
     <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
@@ -5504,7 +5808,7 @@
       <c r="K20" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="L20" s="14" t="s">
+      <c r="L20" s="42" t="s">
         <v>289</v>
       </c>
     </row>
@@ -5539,7 +5843,7 @@
       <c r="K21" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="L21" s="15"/>
+      <c r="L21" s="43"/>
     </row>
     <row r="22" spans="2:12" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
@@ -5572,7 +5876,7 @@
       <c r="K22" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="L22" s="14" t="s">
+      <c r="L22" s="42" t="s">
         <v>305</v>
       </c>
     </row>
@@ -5607,7 +5911,7 @@
       <c r="K23" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="L23" s="15"/>
+      <c r="L23" s="43"/>
     </row>
     <row r="24" spans="2:12" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
@@ -5640,7 +5944,7 @@
       <c r="K24" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="L24" s="14" t="s">
+      <c r="L24" s="42" t="s">
         <v>313</v>
       </c>
     </row>
@@ -5675,7 +5979,7 @@
       <c r="K25" s="8" t="s">
         <v>315</v>
       </c>
-      <c r="L25" s="15"/>
+      <c r="L25" s="43"/>
     </row>
     <row r="26" spans="2:12" ht="142.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="13" t="s">
@@ -5889,17 +6193,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="L20:L21"/>
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="F4:I4"/>
     <mergeCell ref="J4:L4"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="L8:L9"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="L20:L21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5907,10 +6211,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:I30"/>
+  <dimension ref="B1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="F22" sqref="F22:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5922,37 +6226,38 @@
     <col min="7" max="7" width="20.5703125" customWidth="1"/>
     <col min="8" max="8" width="25.28515625" customWidth="1"/>
     <col min="9" max="9" width="39.42578125" customWidth="1"/>
+    <col min="11" max="11" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:9" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="48" t="s">
         <v>176</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="48" t="s">
         <v>355</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="46" t="s">
         <v>172</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="20" t="s">
+      <c r="E2" s="46"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="39" t="s">
         <v>202</v>
       </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="22"/>
-    </row>
-    <row r="3" spans="2:9" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="27" t="s">
+      <c r="H2" s="40"/>
+      <c r="I2" s="41"/>
+    </row>
+    <row r="3" spans="2:11" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="16" t="s">
         <v>175</v>
       </c>
       <c r="G3" s="6" t="s">
@@ -5965,328 +6270,337 @@
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="30" t="s">
+    <row r="4" spans="2:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="18" t="s">
         <v>356</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="20" t="s">
         <v>364</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="42" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="35" t="s">
+      <c r="K4" s="68" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="23" t="s">
         <v>356</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="25" t="s">
         <v>365</v>
       </c>
-      <c r="H5" s="39" t="s">
+      <c r="H5" s="26" t="s">
         <v>223</v>
       </c>
-      <c r="I5" s="15"/>
-    </row>
-    <row r="6" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="40" t="s">
+      <c r="I5" s="43"/>
+      <c r="K5" s="69" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="28" t="s">
         <v>358</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="43" t="s">
+      <c r="E6" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="44" t="s">
+      <c r="F6" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="43">
+      <c r="G6" s="30">
         <v>15137</v>
       </c>
-      <c r="H6" s="44" t="s">
+      <c r="H6" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="44" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="35" t="s">
+      <c r="K6" s="70" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="23" t="s">
         <v>358</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="67" t="s">
         <v>178</v>
       </c>
-      <c r="F7" s="39" t="s">
+      <c r="F7" s="74" t="s">
         <v>190</v>
       </c>
-      <c r="G7" s="43">
+      <c r="G7" s="30">
         <v>15137</v>
       </c>
-      <c r="H7" s="39" t="s">
+      <c r="H7" s="26" t="s">
         <v>226</v>
       </c>
-      <c r="I7" s="17"/>
-    </row>
-    <row r="8" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="40" t="s">
+      <c r="I7" s="45"/>
+    </row>
+    <row r="8" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="28" t="s">
         <v>358</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="44" t="s">
+      <c r="F8" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="G8" s="30" t="s">
         <v>232</v>
       </c>
-      <c r="H8" s="44" t="s">
-        <v>233</v>
-      </c>
-      <c r="I8" s="18" t="s">
+      <c r="H8" s="31" t="s">
+        <v>370</v>
+      </c>
+      <c r="I8" s="37" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="35" t="s">
+    <row r="9" spans="2:11" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="23" t="s">
         <v>358</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="66" t="s">
         <v>179</v>
       </c>
-      <c r="F9" s="39" t="s">
+      <c r="F9" s="74" t="s">
         <v>191</v>
       </c>
-      <c r="G9" s="38" t="s">
+      <c r="G9" s="25" t="s">
         <v>232</v>
       </c>
-      <c r="H9" s="39" t="s">
+      <c r="H9" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="I9" s="19"/>
-    </row>
-    <row r="10" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="40" t="s">
+      <c r="I9" s="38"/>
+    </row>
+    <row r="10" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="28" t="s">
         <v>359</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="67" t="s">
         <v>180</v>
       </c>
-      <c r="F10" s="44" t="s">
+      <c r="F10" s="73" t="s">
         <v>192</v>
       </c>
-      <c r="G10" s="43" t="s">
+      <c r="G10" s="30" t="s">
         <v>247</v>
       </c>
-      <c r="H10" s="44" t="s">
-        <v>248</v>
-      </c>
-      <c r="I10" s="16" t="s">
+      <c r="H10" s="31" t="s">
+        <v>371</v>
+      </c>
+      <c r="I10" s="44" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="35" t="s">
+    <row r="11" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="23" t="s">
         <v>359</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="38" t="s">
+      <c r="E11" s="63" t="s">
         <v>181</v>
       </c>
-      <c r="F11" s="39" t="s">
+      <c r="F11" s="74" t="s">
         <v>193</v>
       </c>
-      <c r="G11" s="38">
+      <c r="G11" s="25">
         <v>1</v>
       </c>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="26" t="s">
         <v>254</v>
       </c>
-      <c r="I11" s="17"/>
-    </row>
-    <row r="12" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="40" t="s">
+      <c r="I11" s="45"/>
+    </row>
+    <row r="12" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="28" t="s">
         <v>359</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="67" t="s">
         <v>182</v>
       </c>
-      <c r="F12" s="44" t="s">
+      <c r="F12" s="73" t="s">
         <v>194</v>
       </c>
-      <c r="G12" s="43" t="s">
+      <c r="G12" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="H12" s="44" t="s">
-        <v>260</v>
-      </c>
-      <c r="I12" s="18" t="s">
+      <c r="H12" s="31" t="s">
+        <v>372</v>
+      </c>
+      <c r="I12" s="37" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="35" t="s">
+    <row r="13" spans="2:11" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="23" t="s">
         <v>359</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="63" t="s">
         <v>183</v>
       </c>
-      <c r="F13" s="39" t="s">
+      <c r="F13" s="75" t="s">
         <v>195</v>
       </c>
-      <c r="G13" s="38" t="s">
+      <c r="G13" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="H13" s="39" t="s">
+      <c r="H13" s="26" t="s">
         <v>266</v>
       </c>
-      <c r="I13" s="19"/>
-    </row>
-    <row r="14" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="40" t="s">
+      <c r="I13" s="38"/>
+    </row>
+    <row r="14" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="28" t="s">
         <v>358</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="E14" s="43" t="s">
+      <c r="E14" s="30" t="s">
         <v>184</v>
       </c>
-      <c r="F14" s="44" t="s">
+      <c r="F14" s="31" t="s">
         <v>196</v>
       </c>
-      <c r="G14" s="43">
+      <c r="G14" s="30">
         <v>1</v>
       </c>
-      <c r="H14" s="44">
+      <c r="H14" s="31">
         <v>38353</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="35" t="s">
+    <row r="15" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="23" t="s">
         <v>358</v>
       </c>
-      <c r="D15" s="37" t="s">
+      <c r="D15" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="E15" s="38" t="s">
+      <c r="E15" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="F15" s="39" t="s">
+      <c r="F15" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="G15" s="38">
+      <c r="G15" s="25">
         <v>1</v>
       </c>
-      <c r="H15" s="39">
+      <c r="H15" s="26">
         <v>38353</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="40" t="s">
+    <row r="16" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="28" t="s">
         <v>358</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="E16" s="43" t="s">
+      <c r="E16" s="30" t="s">
         <v>187</v>
       </c>
-      <c r="F16" s="44" t="s">
+      <c r="F16" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="G16" s="43" t="s">
+      <c r="G16" s="30" t="s">
         <v>277</v>
       </c>
-      <c r="H16" s="44" t="s">
+      <c r="H16" s="31" t="s">
         <v>278</v>
       </c>
       <c r="I16" s="8" t="s">
@@ -6294,25 +6608,25 @@
       </c>
     </row>
     <row r="17" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="23" t="s">
         <v>358</v>
       </c>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="43" t="s">
+      <c r="E17" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="F17" s="39" t="s">
+      <c r="F17" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="G17" s="43" t="s">
+      <c r="G17" s="30" t="s">
         <v>277</v>
       </c>
-      <c r="H17" s="39" t="s">
+      <c r="H17" s="26" t="s">
         <v>278</v>
       </c>
       <c r="I17" s="8" t="s">
@@ -6320,195 +6634,195 @@
       </c>
     </row>
     <row r="18" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="28" t="s">
         <v>358</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="E18" s="43" t="s">
+      <c r="E18" s="64" t="s">
         <v>118</v>
       </c>
-      <c r="F18" s="44" t="s">
+      <c r="F18" s="73" t="s">
         <v>119</v>
       </c>
-      <c r="G18" s="43" t="s">
+      <c r="G18" s="30" t="s">
         <v>287</v>
       </c>
-      <c r="H18" s="44" t="s">
+      <c r="H18" s="31" t="s">
         <v>288</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="I18" s="42" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="23" t="s">
         <v>358</v>
       </c>
-      <c r="D19" s="37" t="s">
+      <c r="D19" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="E19" s="66" t="s">
         <v>128</v>
       </c>
-      <c r="F19" s="39" t="s">
+      <c r="F19" s="74" t="s">
         <v>129</v>
       </c>
-      <c r="G19" s="38" t="s">
+      <c r="G19" s="25" t="s">
         <v>296</v>
       </c>
-      <c r="H19" s="39" t="s">
+      <c r="H19" s="26" t="s">
         <v>297</v>
       </c>
-      <c r="I19" s="15"/>
+      <c r="I19" s="43"/>
     </row>
     <row r="20" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="28" t="s">
         <v>360</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="E20" s="43" t="s">
+      <c r="E20" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="F20" s="44" t="s">
+      <c r="F20" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="G20" s="43" t="s">
+      <c r="G20" s="30" t="s">
         <v>303</v>
       </c>
-      <c r="H20" s="44" t="s">
+      <c r="H20" s="31" t="s">
         <v>304</v>
       </c>
-      <c r="I20" s="14" t="s">
+      <c r="I20" s="42" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="28" t="s">
         <v>360</v>
       </c>
-      <c r="D21" s="37" t="s">
+      <c r="D21" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="E21" s="38" t="s">
+      <c r="E21" s="63" t="s">
         <v>145</v>
       </c>
-      <c r="F21" s="39" t="s">
+      <c r="F21" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="G21" s="38" t="s">
+      <c r="G21" s="25" t="s">
         <v>310</v>
       </c>
-      <c r="H21" s="39" t="s">
+      <c r="H21" s="26" t="s">
         <v>304</v>
       </c>
-      <c r="I21" s="15"/>
+      <c r="I21" s="43"/>
     </row>
     <row r="22" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="C22" s="41" t="s">
+      <c r="C22" s="28" t="s">
         <v>361</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D22" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="E22" s="43" t="s">
+      <c r="E22" s="67" t="s">
         <v>188</v>
       </c>
-      <c r="F22" s="44" t="s">
+      <c r="F22" s="73" t="s">
         <v>188</v>
       </c>
-      <c r="G22" s="43" t="s">
+      <c r="G22" s="30" t="s">
         <v>311</v>
       </c>
-      <c r="H22" s="44" t="s">
+      <c r="H22" s="31" t="s">
         <v>312</v>
       </c>
-      <c r="I22" s="14" t="s">
+      <c r="I22" s="42" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="C23" s="41" t="s">
+      <c r="C23" s="28" t="s">
         <v>361</v>
       </c>
-      <c r="D23" s="37" t="s">
+      <c r="D23" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="E23" s="38" t="s">
+      <c r="E23" s="66" t="s">
         <v>189</v>
       </c>
-      <c r="F23" s="39" t="s">
+      <c r="F23" s="74" t="s">
         <v>189</v>
       </c>
-      <c r="G23" s="38" t="s">
+      <c r="G23" s="25" t="s">
         <v>314</v>
       </c>
-      <c r="H23" s="39" t="s">
+      <c r="H23" s="26" t="s">
         <v>315</v>
       </c>
-      <c r="I23" s="15"/>
+      <c r="I23" s="43"/>
     </row>
     <row r="24" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="27" t="s">
         <v>155</v>
       </c>
-      <c r="C24" s="41" t="s">
+      <c r="C24" s="28" t="s">
         <v>362</v>
       </c>
-      <c r="D24" s="42" t="s">
+      <c r="D24" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="E24" s="43" t="s">
+      <c r="E24" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="F24" s="44" t="s">
+      <c r="F24" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="G24" s="43"/>
-      <c r="H24" s="44"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="31"/>
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="2:9" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="27" t="s">
         <v>316</v>
       </c>
-      <c r="C25" s="41" t="s">
+      <c r="C25" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="D25" s="42" t="s">
+      <c r="D25" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="E25" s="43" t="s">
+      <c r="E25" s="30" t="s">
         <v>350</v>
       </c>
-      <c r="F25" s="44" t="s">
+      <c r="F25" s="31" t="s">
         <v>353</v>
       </c>
-      <c r="G25" s="43" t="s">
+      <c r="G25" s="30" t="s">
         <v>322</v>
       </c>
-      <c r="H25" s="44" t="s">
+      <c r="H25" s="31" t="s">
         <v>323</v>
       </c>
       <c r="I25" s="8" t="s">
@@ -6516,25 +6830,25 @@
       </c>
     </row>
     <row r="26" spans="2:9" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="27" t="s">
         <v>325</v>
       </c>
-      <c r="C26" s="41" t="s">
+      <c r="C26" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="D26" s="42" t="s">
+      <c r="D26" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="E26" s="43" t="s">
+      <c r="E26" s="30" t="s">
         <v>351</v>
       </c>
-      <c r="F26" s="44" t="s">
+      <c r="F26" s="31" t="s">
         <v>353</v>
       </c>
-      <c r="G26" s="43" t="s">
+      <c r="G26" s="30" t="s">
         <v>329</v>
       </c>
-      <c r="H26" s="44" t="s">
+      <c r="H26" s="31" t="s">
         <v>330</v>
       </c>
       <c r="I26" s="8" t="s">
@@ -6542,25 +6856,25 @@
       </c>
     </row>
     <row r="27" spans="2:9" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="27" t="s">
         <v>332</v>
       </c>
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="28" t="s">
         <v>363</v>
       </c>
-      <c r="D27" s="42" t="s">
+      <c r="D27" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="E27" s="43" t="s">
+      <c r="E27" s="30" t="s">
         <v>352</v>
       </c>
-      <c r="F27" s="44" t="s">
+      <c r="F27" s="31" t="s">
         <v>354</v>
       </c>
-      <c r="G27" s="43" t="s">
+      <c r="G27" s="30" t="s">
         <v>366</v>
       </c>
-      <c r="H27" s="44" t="s">
+      <c r="H27" s="31" t="s">
         <v>336</v>
       </c>
       <c r="I27" s="8" t="s">
@@ -6568,25 +6882,25 @@
       </c>
     </row>
     <row r="28" spans="2:9" ht="99.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="C28" s="36" t="s">
+      <c r="C28" s="23" t="s">
         <v>363</v>
       </c>
-      <c r="D28" s="37" t="s">
+      <c r="D28" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="E28" s="38" t="s">
+      <c r="E28" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="F28" s="39" t="s">
+      <c r="F28" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="G28" s="38" t="s">
+      <c r="G28" s="25" t="s">
         <v>367</v>
       </c>
-      <c r="H28" s="39" t="s">
+      <c r="H28" s="26" t="s">
         <v>336</v>
       </c>
       <c r="I28" s="8" t="s">
@@ -6594,25 +6908,25 @@
       </c>
     </row>
     <row r="29" spans="2:9" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="C29" s="41" t="s">
+      <c r="C29" s="28" t="s">
         <v>363</v>
       </c>
-      <c r="D29" s="42" t="s">
+      <c r="D29" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="E29" s="43" t="s">
+      <c r="E29" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="F29" s="44" t="s">
+      <c r="F29" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="G29" s="43" t="s">
+      <c r="G29" s="30" t="s">
         <v>368</v>
       </c>
-      <c r="H29" s="44" t="s">
+      <c r="H29" s="31" t="s">
         <v>336</v>
       </c>
       <c r="I29" s="8" t="s">
@@ -6620,25 +6934,25 @@
       </c>
     </row>
     <row r="30" spans="2:9" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="45" t="s">
+      <c r="B30" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="C30" s="46" t="s">
+      <c r="C30" s="33" t="s">
         <v>363</v>
       </c>
-      <c r="D30" s="47" t="s">
+      <c r="D30" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="E30" s="48" t="s">
+      <c r="E30" s="35" t="s">
         <v>161</v>
       </c>
-      <c r="F30" s="49" t="s">
+      <c r="F30" s="36" t="s">
         <v>170</v>
       </c>
-      <c r="G30" s="48" t="s">
+      <c r="G30" s="35" t="s">
         <v>369</v>
       </c>
-      <c r="H30" s="49" t="s">
+      <c r="H30" s="36" t="s">
         <v>336</v>
       </c>
       <c r="I30" s="8" t="s">
@@ -6647,22 +6961,1365 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="I10:I11"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB69EAB-8C05-4507-AE10-22616E6C1D6E}">
+  <dimension ref="B2:P31"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:P31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="21" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" customWidth="1"/>
+    <col min="16" max="16" width="26.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>355</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="H3" s="51"/>
+      <c r="J3" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="K3" s="48" t="s">
+        <v>355</v>
+      </c>
+      <c r="L3" s="46" t="s">
+        <v>172</v>
+      </c>
+      <c r="M3" s="46"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="P3" s="51"/>
+    </row>
+    <row r="4" spans="2:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="J4" s="49"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="52" t="s">
+        <v>173</v>
+      </c>
+      <c r="M4" s="58" t="s">
+        <v>174</v>
+      </c>
+      <c r="N4" s="59" t="s">
+        <v>175</v>
+      </c>
+      <c r="O4" s="60" t="s">
+        <v>210</v>
+      </c>
+      <c r="P4" s="60" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="20">
+        <v>1.12E-2</v>
+      </c>
+      <c r="F5" s="21">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>364</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="61" t="s">
+        <v>356</v>
+      </c>
+      <c r="L5" s="20">
+        <f>ROUND(D5,4)</f>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="M5" s="20">
+        <f>ROUND(E5,4)</f>
+        <v>1.12E-2</v>
+      </c>
+      <c r="N5" s="20">
+        <f>ROUND(F5,4)</f>
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="O5" s="20" t="s">
+        <v>364</v>
+      </c>
+      <c r="P5" s="21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>356</v>
+      </c>
+      <c r="D6" s="24">
+        <v>1.7600000000000001E-3</v>
+      </c>
+      <c r="E6" s="25">
+        <v>4.6999999999999999E-4</v>
+      </c>
+      <c r="F6" s="26">
+        <v>2.5600000000000002E-3</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>365</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="23" t="s">
+        <v>356</v>
+      </c>
+      <c r="L6" s="30">
+        <f t="shared" ref="L6:L20" si="0">ROUND(D6,4)</f>
+        <v>1.8E-3</v>
+      </c>
+      <c r="M6" s="30">
+        <f t="shared" ref="M6:M20" si="1">ROUND(E6,4)</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="N6" s="30">
+        <f t="shared" ref="N6:N20" si="2">ROUND(F6,4)</f>
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="O6" s="25" t="s">
+        <v>365</v>
+      </c>
+      <c r="P6" s="26" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>358</v>
+      </c>
+      <c r="D7" s="29">
+        <v>2.0489999999999999</v>
+      </c>
+      <c r="E7" s="30">
+        <v>1.4870000000000001</v>
+      </c>
+      <c r="F7" s="31">
+        <v>1.5009999999999999</v>
+      </c>
+      <c r="G7" s="30">
+        <v>15137</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="J7" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>358</v>
+      </c>
+      <c r="L7" s="30">
+        <f t="shared" si="0"/>
+        <v>2.0489999999999999</v>
+      </c>
+      <c r="M7" s="30">
+        <f t="shared" si="1"/>
+        <v>1.4870000000000001</v>
+      </c>
+      <c r="N7" s="30">
+        <f t="shared" si="2"/>
+        <v>1.5009999999999999</v>
+      </c>
+      <c r="O7" s="30">
+        <v>15137</v>
+      </c>
+      <c r="P7" s="31" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>358</v>
+      </c>
+      <c r="D8" s="24">
+        <v>2.05002</v>
+      </c>
+      <c r="E8" s="30">
+        <v>2.03478</v>
+      </c>
+      <c r="F8" s="26">
+        <v>1.4845900000000001</v>
+      </c>
+      <c r="G8" s="30">
+        <v>15137</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="J8" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="23" t="s">
+        <v>358</v>
+      </c>
+      <c r="L8" s="30">
+        <f t="shared" si="0"/>
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="M8" s="30">
+        <f t="shared" si="1"/>
+        <v>2.0348000000000002</v>
+      </c>
+      <c r="N8" s="30">
+        <f t="shared" si="2"/>
+        <v>1.4845999999999999</v>
+      </c>
+      <c r="O8" s="30">
+        <v>15137</v>
+      </c>
+      <c r="P8" s="26" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>358</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="J9" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>358</v>
+      </c>
+      <c r="L9" s="30">
+        <f t="shared" si="0"/>
+        <v>0.2278</v>
+      </c>
+      <c r="M9" s="30">
+        <f t="shared" si="1"/>
+        <v>0.1789</v>
+      </c>
+      <c r="N9" s="30">
+        <f t="shared" si="2"/>
+        <v>0.13469999999999999</v>
+      </c>
+      <c r="O9" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="P9" s="31" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>358</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="25">
+        <v>0.276669</v>
+      </c>
+      <c r="F10" s="26">
+        <v>0.156116</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="H10" s="26" t="s">
+        <v>241</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10" s="23" t="s">
+        <v>358</v>
+      </c>
+      <c r="L10" s="30">
+        <f t="shared" si="0"/>
+        <v>0.16170000000000001</v>
+      </c>
+      <c r="M10" s="30">
+        <f t="shared" si="1"/>
+        <v>0.2767</v>
+      </c>
+      <c r="N10" s="30">
+        <f t="shared" si="2"/>
+        <v>0.15609999999999999</v>
+      </c>
+      <c r="O10" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="P10" s="26" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>359</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="30">
+        <v>0.76925900000000003</v>
+      </c>
+      <c r="F11" s="31">
+        <v>0.49195499999999998</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="J11" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="K11" s="28" t="s">
+        <v>359</v>
+      </c>
+      <c r="L11" s="30">
+        <f t="shared" si="0"/>
+        <v>0.44219999999999998</v>
+      </c>
+      <c r="M11" s="30">
+        <f t="shared" si="1"/>
+        <v>0.76929999999999998</v>
+      </c>
+      <c r="N11" s="30">
+        <f t="shared" si="2"/>
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="O11" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="P11" s="31" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>359</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="25">
+        <v>0.23802599999999999</v>
+      </c>
+      <c r="F12" s="26">
+        <v>0.938164</v>
+      </c>
+      <c r="G12" s="25">
+        <v>1</v>
+      </c>
+      <c r="H12" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="J12" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="K12" s="23" t="s">
+        <v>359</v>
+      </c>
+      <c r="L12" s="30">
+        <f t="shared" si="0"/>
+        <v>0.95179999999999998</v>
+      </c>
+      <c r="M12" s="30">
+        <f t="shared" si="1"/>
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="N12" s="30">
+        <f t="shared" si="2"/>
+        <v>0.93820000000000003</v>
+      </c>
+      <c r="O12" s="25">
+        <v>1</v>
+      </c>
+      <c r="P12" s="26" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B13" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>359</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="30">
+        <v>0.115755</v>
+      </c>
+      <c r="F13" s="31">
+        <v>0.120658</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>260</v>
+      </c>
+      <c r="J13" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="K13" s="28" t="s">
+        <v>359</v>
+      </c>
+      <c r="L13" s="30">
+        <f t="shared" si="0"/>
+        <v>0.1036</v>
+      </c>
+      <c r="M13" s="30">
+        <f t="shared" si="1"/>
+        <v>0.1158</v>
+      </c>
+      <c r="N13" s="30">
+        <f t="shared" si="2"/>
+        <v>0.1207</v>
+      </c>
+      <c r="O13" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="P13" s="31" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B14" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>359</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="25">
+        <v>1.1450800000000001</v>
+      </c>
+      <c r="F14" s="26">
+        <v>0.98440000000000005</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>265</v>
+      </c>
+      <c r="H14" s="26" t="s">
+        <v>266</v>
+      </c>
+      <c r="J14" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="K14" s="23" t="s">
+        <v>359</v>
+      </c>
+      <c r="L14" s="30">
+        <f t="shared" si="0"/>
+        <v>0.98419999999999996</v>
+      </c>
+      <c r="M14" s="30">
+        <f t="shared" si="1"/>
+        <v>1.1451</v>
+      </c>
+      <c r="N14" s="30">
+        <f t="shared" si="2"/>
+        <v>0.98440000000000005</v>
+      </c>
+      <c r="O14" s="25" t="s">
+        <v>265</v>
+      </c>
+      <c r="P14" s="26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>358</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="30">
+        <v>0.91046000000000005</v>
+      </c>
+      <c r="F15" s="31">
+        <v>1.49655</v>
+      </c>
+      <c r="G15" s="30">
+        <v>1</v>
+      </c>
+      <c r="H15" s="31">
+        <v>38353</v>
+      </c>
+      <c r="J15" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="K15" s="28" t="s">
+        <v>358</v>
+      </c>
+      <c r="L15" s="30">
+        <f t="shared" si="0"/>
+        <v>1.5051000000000001</v>
+      </c>
+      <c r="M15" s="30">
+        <f t="shared" si="1"/>
+        <v>0.91049999999999998</v>
+      </c>
+      <c r="N15" s="30">
+        <f t="shared" si="2"/>
+        <v>1.4965999999999999</v>
+      </c>
+      <c r="O15" s="30">
+        <v>1</v>
+      </c>
+      <c r="P15" s="31">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>358</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="25">
+        <v>1.66879</v>
+      </c>
+      <c r="F16" s="26">
+        <v>1.49909</v>
+      </c>
+      <c r="G16" s="25">
+        <v>1</v>
+      </c>
+      <c r="H16" s="26">
+        <v>38353</v>
+      </c>
+      <c r="J16" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="K16" s="23" t="s">
+        <v>358</v>
+      </c>
+      <c r="L16" s="30">
+        <f t="shared" si="0"/>
+        <v>1.4994000000000001</v>
+      </c>
+      <c r="M16" s="30">
+        <f t="shared" si="1"/>
+        <v>1.6688000000000001</v>
+      </c>
+      <c r="N16" s="30">
+        <f t="shared" si="2"/>
+        <v>1.4991000000000001</v>
+      </c>
+      <c r="O16" s="25">
+        <v>1</v>
+      </c>
+      <c r="P16" s="26">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>358</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="30">
+        <v>0.12173399999999999</v>
+      </c>
+      <c r="F17" s="31">
+        <v>0.47713800000000001</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="J17" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="K17" s="28" t="s">
+        <v>358</v>
+      </c>
+      <c r="L17" s="30">
+        <f t="shared" si="0"/>
+        <v>0.48580000000000001</v>
+      </c>
+      <c r="M17" s="30">
+        <f t="shared" si="1"/>
+        <v>0.1217</v>
+      </c>
+      <c r="N17" s="30">
+        <f t="shared" si="2"/>
+        <v>0.47710000000000002</v>
+      </c>
+      <c r="O17" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="P17" s="31" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>358</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="30">
+        <v>1.15541</v>
+      </c>
+      <c r="F18" s="26">
+        <v>0.69920000000000004</v>
+      </c>
+      <c r="G18" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="H18" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="J18" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="K18" s="23" t="s">
+        <v>358</v>
+      </c>
+      <c r="L18" s="30">
+        <f t="shared" si="0"/>
+        <v>0.69889999999999997</v>
+      </c>
+      <c r="M18" s="30">
+        <f t="shared" si="1"/>
+        <v>1.1554</v>
+      </c>
+      <c r="N18" s="30">
+        <f t="shared" si="2"/>
+        <v>0.69920000000000004</v>
+      </c>
+      <c r="O18" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="P18" s="26" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>358</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="G19" s="30" t="s">
+        <v>287</v>
+      </c>
+      <c r="H19" s="31" t="s">
+        <v>288</v>
+      </c>
+      <c r="J19" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="K19" s="28" t="s">
+        <v>358</v>
+      </c>
+      <c r="L19" s="30">
+        <f t="shared" si="0"/>
+        <v>0.63829999999999998</v>
+      </c>
+      <c r="M19" s="30">
+        <f t="shared" si="1"/>
+        <v>0.42149999999999999</v>
+      </c>
+      <c r="N19" s="30">
+        <f t="shared" si="2"/>
+        <v>0.64659999999999995</v>
+      </c>
+      <c r="O19" s="30" t="s">
+        <v>287</v>
+      </c>
+      <c r="P19" s="31" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>358</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>296</v>
+      </c>
+      <c r="H20" s="26" t="s">
+        <v>297</v>
+      </c>
+      <c r="J20" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="K20" s="23" t="s">
+        <v>358</v>
+      </c>
+      <c r="L20" s="30">
+        <f t="shared" si="0"/>
+        <v>0.48159999999999997</v>
+      </c>
+      <c r="M20" s="30">
+        <f t="shared" si="1"/>
+        <v>0.36230000000000001</v>
+      </c>
+      <c r="N20" s="30">
+        <f t="shared" si="2"/>
+        <v>0.48320000000000002</v>
+      </c>
+      <c r="O20" s="25" t="s">
+        <v>296</v>
+      </c>
+      <c r="P20" s="26" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>360</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="G21" s="30" t="s">
+        <v>303</v>
+      </c>
+      <c r="H21" s="31" t="s">
+        <v>304</v>
+      </c>
+      <c r="J21" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="K21" s="28" t="s">
+        <v>360</v>
+      </c>
+      <c r="L21" s="54">
+        <v>1.337E-11</v>
+      </c>
+      <c r="M21" s="55">
+        <v>1.336E-11</v>
+      </c>
+      <c r="N21" s="56">
+        <v>9.3559999999999998E-11</v>
+      </c>
+      <c r="O21" s="30" t="s">
+        <v>303</v>
+      </c>
+      <c r="P21" s="31" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>360</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>310</v>
+      </c>
+      <c r="H22" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="J22" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="K22" s="28" t="s">
+        <v>360</v>
+      </c>
+      <c r="L22" s="53" t="s">
+        <v>144</v>
+      </c>
+      <c r="M22" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="N22" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="O22" s="25" t="s">
+        <v>310</v>
+      </c>
+      <c r="P22" s="26" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>361</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="E23" s="30">
+        <v>900</v>
+      </c>
+      <c r="F23" s="31">
+        <v>900</v>
+      </c>
+      <c r="G23" s="30" t="s">
+        <v>311</v>
+      </c>
+      <c r="H23" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="J23" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="K23" s="28" t="s">
+        <v>361</v>
+      </c>
+      <c r="L23" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="M23" s="30">
+        <v>900</v>
+      </c>
+      <c r="N23" s="31">
+        <v>900</v>
+      </c>
+      <c r="O23" s="30" t="s">
+        <v>311</v>
+      </c>
+      <c r="P23" s="31" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>361</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="E24" s="25">
+        <v>1900</v>
+      </c>
+      <c r="F24" s="26">
+        <v>1900</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>314</v>
+      </c>
+      <c r="H24" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="J24" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="K24" s="28" t="s">
+        <v>361</v>
+      </c>
+      <c r="L24" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="M24" s="25">
+        <v>1900</v>
+      </c>
+      <c r="N24" s="26">
+        <v>1900</v>
+      </c>
+      <c r="O24" s="25" t="s">
+        <v>314</v>
+      </c>
+      <c r="P24" s="26" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>362</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="F25" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="G25" s="30"/>
+      <c r="H25" s="31"/>
+      <c r="J25" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="K25" s="28" t="s">
+        <v>362</v>
+      </c>
+      <c r="L25" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="M25" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="N25" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="O25" s="30"/>
+      <c r="P25" s="31"/>
+    </row>
+    <row r="26" spans="2:16" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="27" t="s">
+        <v>316</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="E26" s="30">
+        <v>0.151477</v>
+      </c>
+      <c r="F26" s="31">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G26" s="30" t="s">
+        <v>322</v>
+      </c>
+      <c r="H26" s="31" t="s">
+        <v>323</v>
+      </c>
+      <c r="J26" s="27" t="s">
+        <v>316</v>
+      </c>
+      <c r="K26" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="L26" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="M26" s="30">
+        <f>ROUND(E26,4)</f>
+        <v>0.1515</v>
+      </c>
+      <c r="N26" s="30">
+        <f>ROUND(F26,4)</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="O26" s="30" t="s">
+        <v>322</v>
+      </c>
+      <c r="P26" s="31" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="27" t="s">
+        <v>325</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="E27" s="30">
+        <v>0.87941899999999995</v>
+      </c>
+      <c r="F27" s="31">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G27" s="30" t="s">
+        <v>329</v>
+      </c>
+      <c r="H27" s="31" t="s">
+        <v>330</v>
+      </c>
+      <c r="J27" s="27" t="s">
+        <v>325</v>
+      </c>
+      <c r="K27" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="L27" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="M27" s="30">
+        <f t="shared" ref="M27:M31" si="3">ROUND(E27,4)</f>
+        <v>0.87939999999999996</v>
+      </c>
+      <c r="N27" s="30">
+        <f t="shared" ref="N27:N31" si="4">ROUND(F27,4)</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="O27" s="30" t="s">
+        <v>329</v>
+      </c>
+      <c r="P27" s="31" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>363</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="E28" s="30">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="F28" s="31">
+        <v>0.01</v>
+      </c>
+      <c r="G28" s="30" t="s">
+        <v>366</v>
+      </c>
+      <c r="H28" s="31" t="s">
+        <v>336</v>
+      </c>
+      <c r="J28" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="K28" s="28" t="s">
+        <v>363</v>
+      </c>
+      <c r="L28" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="M28" s="30">
+        <f t="shared" si="3"/>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="N28" s="30">
+        <f t="shared" si="4"/>
+        <v>0.01</v>
+      </c>
+      <c r="O28" s="30" t="s">
+        <v>366</v>
+      </c>
+      <c r="P28" s="31" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>363</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="F29" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>367</v>
+      </c>
+      <c r="H29" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="J29" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="K29" s="23" t="s">
+        <v>363</v>
+      </c>
+      <c r="L29" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="M29" s="30">
+        <f t="shared" si="3"/>
+        <v>0.02</v>
+      </c>
+      <c r="N29" s="30">
+        <f t="shared" si="4"/>
+        <v>2.07E-2</v>
+      </c>
+      <c r="O29" s="25" t="s">
+        <v>367</v>
+      </c>
+      <c r="P29" s="26" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>363</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="F30" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="G30" s="30" t="s">
+        <v>368</v>
+      </c>
+      <c r="H30" s="31" t="s">
+        <v>336</v>
+      </c>
+      <c r="J30" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="K30" s="28" t="s">
+        <v>363</v>
+      </c>
+      <c r="L30" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="M30" s="30">
+        <f t="shared" si="3"/>
+        <v>4.3099999999999999E-2</v>
+      </c>
+      <c r="N30" s="30">
+        <f t="shared" si="4"/>
+        <v>4.0399999999999998E-2</v>
+      </c>
+      <c r="O30" s="30" t="s">
+        <v>368</v>
+      </c>
+      <c r="P30" s="31" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>363</v>
+      </c>
+      <c r="D31" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="E31" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="F31" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="G31" s="35" t="s">
+        <v>369</v>
+      </c>
+      <c r="H31" s="36" t="s">
+        <v>336</v>
+      </c>
+      <c r="J31" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="K31" s="33" t="s">
+        <v>363</v>
+      </c>
+      <c r="L31" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="M31" s="62">
+        <f t="shared" si="3"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N31" s="62">
+        <f t="shared" si="4"/>
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="O31" s="35" t="s">
+        <v>369</v>
+      </c>
+      <c r="P31" s="36" t="s">
+        <v>336</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:H3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>